<commit_message>
added outer rooms and changed color to blue
</commit_message>
<xml_diff>
--- a/school map app coordinates.xlsx
+++ b/school map app coordinates.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14505" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="14505" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="223">
   <si>
     <t>Name</t>
   </si>
@@ -574,9 +574,6 @@
     <t>2,6</t>
   </si>
   <si>
-    <t xml:space="preserve"> 4,1,2,1,4,8,4,10,4,18,2,18,2,8,2,10</t>
-  </si>
-  <si>
     <t>4,4</t>
   </si>
   <si>
@@ -674,6 +671,33 @@
   </si>
   <si>
     <t>Stair</t>
+  </si>
+  <si>
+    <t>outerRoom</t>
+  </si>
+  <si>
+    <t>Storage1</t>
+  </si>
+  <si>
+    <t>Stairs1</t>
+  </si>
+  <si>
+    <t>Stairs2</t>
+  </si>
+  <si>
+    <t>OuterRoom</t>
+  </si>
+  <si>
+    <t>309</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,1,2,2,4,8,4,10,4,18,2,18,2,8,2,10,1,30,1,2</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Admin Office</t>
   </si>
 </sst>
 </file>
@@ -4169,22 +4193,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:K149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57.875" customWidth="1"/>
-    <col min="9" max="9" width="18.875" customWidth="1"/>
-    <col min="10" max="10" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="42.5" customWidth="1"/>
+    <col min="9" max="9" width="57.875" customWidth="1"/>
+    <col min="10" max="10" width="18.875" customWidth="1"/>
+    <col min="11" max="11" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4206,14 +4231,17 @@
       <c r="G1" t="s">
         <v>165</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>164</v>
       </c>
@@ -4235,15 +4263,15 @@
       <c r="G2" t="s">
         <v>166</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE(" new Room('", A2,"', ", B2,", ", C2,", ",D2,", ",E2, ",[",F2,"],'",G2,"'),")</f>
-        <v xml:space="preserve"> new Room('mech3', 0, 4, 13, 9,[2,3],'Normal'),</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="I2" t="str">
+        <f>CONCATENATE(" new Room('", A2,"', ", B2,", ", C2,", ",D2,", ",E2, ",[",F2,"],'",G2,"','",H2,"'),")</f>
+        <v xml:space="preserve"> new Room('mech3', 0, 4, 13, 9,[2,3],'Normal',''),</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -4265,15 +4293,15 @@
       <c r="G3" t="s">
         <v>166</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H62" si="0">CONCATENATE(" new Room('", A3,"', ", B3,", ", C3,", ",D3,", ",E3, ",[",F3,"],'",G3,"'),")</f>
-        <v xml:space="preserve"> new Room('receiving', 5, 13, 8, 5,[2,4],'Normal'),</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I6" si="0">CONCATENATE(" new Room('", A3,"', ", B3,", ", C3,", ",D3,", ",E3, ",[",F3,"],'",G3,"','",H3,"'),")</f>
+        <v xml:space="preserve"> new Room('receiving', 5, 13, 8, 5,[2,4],'Normal',''),</v>
+      </c>
+      <c r="K3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -4295,15 +4323,15 @@
       <c r="G4" t="s">
         <v>166</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('kitchen', 2, 18, 11, 10,[3,1],'Normal'),</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('kitchen', 2, 18, 11, 10,[3,1],'Normal',''),</v>
+      </c>
+      <c r="K4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -4325,15 +4353,15 @@
       <c r="G5" t="s">
         <v>166</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('servery', 2, 28, 8, 9,[2,9],'Normal'),</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('servery', 2, 28, 8, 9,[2,9],'Normal',''),</v>
+      </c>
+      <c r="K5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -4355,15 +4383,15 @@
       <c r="G6" t="s">
         <v>166</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('faculty lounge', 2, 37, 8, 6,[2,6],'Normal'),</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('faculty lounge', 2, 37, 8, 6,[2,6],'Normal',''),</v>
+      </c>
+      <c r="K6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -4380,20 +4408,20 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="G8" t="s">
         <v>166</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('main gym', 16, 23, 32, 18,[ 4,1,2,1,4,8,4,10,4,18,2,18,2,8,2,10],'Normal'),</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" t="str">
+        <f t="shared" ref="I8:I10" si="1">CONCATENATE(" new Room('", A8,"', ", B8,", ", C8,", ",D8,", ",E8, ",[",F8,"],'",G8,"','",H8,"'),")</f>
+        <v xml:space="preserve"> new Room('main gym', 16, 23, 32, 18,[ 4,1,2,2,4,8,4,10,4,18,2,18,2,8,2,10,1,30,1,2],'Normal',''),</v>
+      </c>
+      <c r="K8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -4415,15 +4443,18 @@
       <c r="G9" t="s">
         <v>166</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('boys locker', 16, 17, 16, 6,[3,2],'Normal'),</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Room('boys locker', 16, 17, 16, 6,[3,2],'Normal','main gym'),</v>
+      </c>
+      <c r="K9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -4440,20 +4471,23 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" t="s">
         <v>166</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('girls locker', 32, 17, 16, 6,[3,14],'Normal'),</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Room('girls locker', 32, 17, 16, 6,[3,14],'Normal','main gym'),</v>
+      </c>
+      <c r="K10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -4470,20 +4504,20 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G12" t="s">
         <v>166</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('trainer\'s room', 16, 7, 5, 5,[4,4],'Normal'),</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="I12" t="str">
+        <f t="shared" ref="I12:I16" si="2">CONCATENATE(" new Room('", A12,"', ", B12,", ", C12,", ",D12,", ",E12, ",[",F12,"],'",G12,"','",H12,"'),")</f>
+        <v xml:space="preserve"> new Room('trainer\'s room', 16, 7, 5, 5,[4,4],'Normal',''),</v>
+      </c>
+      <c r="K12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -4502,15 +4536,15 @@
       <c r="G13" t="s">
         <v>166</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('team room 1', 21, 7, 16, 8,[],'Normal'),</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="I13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('team room 1', 21, 7, 16, 8,[],'Normal',''),</v>
+      </c>
+      <c r="K13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -4529,15 +4563,15 @@
       <c r="G14" t="s">
         <v>166</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('team room 2', 39, 7, 9, 8,[],'Normal'),</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('team room 2', 39, 7, 9, 8,[],'Normal',''),</v>
+      </c>
+      <c r="K14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>35</v>
       </c>
@@ -4554,20 +4588,20 @@
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G15" t="s">
         <v>166</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('606', 50, 7, 13, 9,[4,9,2,2],'Normal'),</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('606', 50, 7, 13, 9,[4,9,2,2],'Normal',''),</v>
+      </c>
+      <c r="K15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -4584,20 +4618,20 @@
         <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G16" t="s">
         <v>166</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('602', 63, 8, 10, 8,[3,1,2,1],'Normal'),</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('602', 63, 8, 10, 8,[3,1,2,1],'Normal',''),</v>
+      </c>
+      <c r="K16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>151</v>
       </c>
@@ -4616,13 +4650,13 @@
       <c r="G18" t="s">
         <v>173</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('cafeteria', 16, 43, 32, 11,[],'Walkable'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <f>CONCATENATE(" new Room('", A18,"', ", B18,", ", C18,", ",D18,", ",E18, ",[",F18,"],'",G18,"','",H18,"'),")</f>
+        <v xml:space="preserve"> new Room('cafeteria', 16, 43, 32, 11,[],'Walkable',''),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
@@ -4641,18 +4675,18 @@
       <c r="G20" t="s">
         <v>166</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
+      <c r="I20" t="str">
+        <f t="shared" ref="I20:I22" si="3">CONCATENATE(" new Room('", A20,"', ", B20,", ", C20,", ",D20,", ",E20, ",[",F20,"],'",G20,"'),")</f>
         <v xml:space="preserve"> new Room('band room', 1, 57, 12, 9,[],'Normal'),</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>105</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -4671,18 +4705,18 @@
       <c r="G21" t="s">
         <v>166</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
+      <c r="I21" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> new Room('orchestra', 0, 74, 13, 9,[],'Normal'),</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>106</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -4701,18 +4735,18 @@
       <c r="G22" t="s">
         <v>166</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
+      <c r="I22" t="str">
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> new Room('choir', 25, 77, 13, 9,[],'Normal'),</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>108</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>34</v>
       </c>
@@ -4729,20 +4763,20 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G23" t="s">
         <v>166</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('school store', 55, 46, 5, 5,[4,2],'Normal'),</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="I23" t="str">
+        <f>CONCATENATE(" new Room('", A23,"', ", B23,", ", C23,", ",D23,", ",E23, ",[",F23,"],'",G23,"','",H23,"'),")</f>
+        <v xml:space="preserve"> new Room('school store', 55, 46, 5, 5,[4,2],'Normal',''),</v>
+      </c>
+      <c r="K23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>152</v>
       </c>
@@ -4759,20 +4793,20 @@
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" t="s">
         <v>166</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('mech1', 63, 0, 6, 5,[4,3],'Normal'),</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I25" t="str">
+        <f t="shared" ref="I25:I33" si="4">CONCATENATE(" new Room('", A25,"', ", B25,", ", C25,", ",D25,", ",E25, ",[",F25,"],'",G25,"','",H25,"'),")</f>
+        <v xml:space="preserve"> new Room('mech1', 63, 0, 6, 5,[4,3],'Normal',''),</v>
+      </c>
+      <c r="K25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>153</v>
       </c>
@@ -4794,15 +4828,15 @@
       <c r="G26" t="s">
         <v>166</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('mech2', 69, 0, 6, 5,[3,2],'Normal'),</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="I26" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('mech2', 69, 0, 6, 5,[3,2],'Normal',''),</v>
+      </c>
+      <c r="K26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
@@ -4819,20 +4853,20 @@
         <v>5</v>
       </c>
       <c r="F27" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G27" t="s">
         <v>166</v>
       </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('210', 75, 0, 8, 5,[3,7],'Normal'),</v>
-      </c>
-      <c r="J27">
+      <c r="I27" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('210', 75, 0, 8, 5,[3,7],'Normal',''),</v>
+      </c>
+      <c r="K27">
         <v>150</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>41</v>
       </c>
@@ -4854,15 +4888,15 @@
       <c r="G28" t="s">
         <v>166</v>
       </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('211', 83, 0, 8, 5,[3,2],'Normal'),</v>
-      </c>
-      <c r="J28">
+      <c r="I28" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('211', 83, 0, 8, 5,[3,2],'Normal',''),</v>
+      </c>
+      <c r="K28">
         <v>148</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>42</v>
       </c>
@@ -4879,20 +4913,20 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G29" t="s">
         <v>166</v>
       </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('212', 91, 0, 9, 5,[3,7],'Normal'),</v>
-      </c>
-      <c r="J29">
+      <c r="I29" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('212', 91, 0, 9, 5,[3,7],'Normal',''),</v>
+      </c>
+      <c r="K29">
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
@@ -4914,15 +4948,15 @@
       <c r="G30" t="s">
         <v>166</v>
       </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('213', 100, 0, 8, 5,[3,2],'Normal'),</v>
-      </c>
-      <c r="J30">
+      <c r="I30" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('213', 100, 0, 8, 5,[3,2],'Normal',''),</v>
+      </c>
+      <c r="K30">
         <v>144</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>44</v>
       </c>
@@ -4939,20 +4973,20 @@
         <v>5</v>
       </c>
       <c r="F31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G31" t="s">
         <v>166</v>
       </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('214', 108, 0, 8, 5,[3,7],'Normal'),</v>
-      </c>
-      <c r="J31">
+      <c r="I31" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('214', 108, 0, 8, 5,[3,7],'Normal',''),</v>
+      </c>
+      <c r="K31">
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
@@ -4974,15 +5008,15 @@
       <c r="G32" t="s">
         <v>166</v>
       </c>
-      <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('215', 116, 0, 8, 5,[3,2],'Normal'),</v>
-      </c>
-      <c r="J32">
+      <c r="I32" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('215', 116, 0, 8, 5,[3,2],'Normal',''),</v>
+      </c>
+      <c r="K32">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>56</v>
       </c>
@@ -5004,15 +5038,15 @@
       <c r="G33" t="s">
         <v>166</v>
       </c>
-      <c r="H33" t="str">
-        <f>CONCATENATE(" new Room('", A33,"', ", B33,", ", C33,", ",D33,", ",E33, ",[",F33,"],'",G33,"'),")</f>
-        <v xml:space="preserve"> new Room('218', 130, 0, 13, 5,[3,2],'Normal'),</v>
-      </c>
-      <c r="J33">
+      <c r="I33" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> new Room('218', 130, 0, 13, 5,[3,2],'Normal',''),</v>
+      </c>
+      <c r="K33">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>131</v>
       </c>
@@ -5031,12 +5065,12 @@
       <c r="G35" t="s">
         <v>166</v>
       </c>
-      <c r="H35" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('131', 71, 58, 9, 6,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" t="str">
+        <f t="shared" ref="I35:I42" si="5">CONCATENATE(" new Room('", A35,"', ", B35,", ", C35,", ",D35,", ",E35, ",[",F35,"],'",G35,"','",H35,"'),")</f>
+        <v xml:space="preserve"> new Room('131', 71, 58, 9, 6,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>133</v>
       </c>
@@ -5055,12 +5089,12 @@
       <c r="G36" t="s">
         <v>166</v>
       </c>
-      <c r="H36" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('133', 80, 58, 8, 6,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('133', 80, 58, 8, 6,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
@@ -5079,12 +5113,12 @@
       <c r="G37" t="s">
         <v>166</v>
       </c>
-      <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Media Center', 71, 64, 17, 15,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Media Center', 71, 64, 17, 15,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>104</v>
       </c>
@@ -5103,12 +5137,12 @@
       <c r="G38" t="s">
         <v>166</v>
       </c>
-      <c r="H38" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Attendance', 84, 81, 7, 4,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Attendance', 84, 81, 7, 4,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>102</v>
       </c>
@@ -5127,12 +5161,12 @@
       <c r="G39" t="s">
         <v>166</v>
       </c>
-      <c r="H39" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Main Office', 69, 80, 7, 6,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Main Office', 69, 80, 7, 6,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>106</v>
       </c>
@@ -5151,12 +5185,12 @@
       <c r="G40" t="s">
         <v>166</v>
       </c>
-      <c r="H40" t="str">
-        <f>CONCATENATE(" new Room('", A40,"', ", B40,", ", C40,", ",D40,", ",E40, ",[",F40,"],'",G40,"'),")</f>
-        <v xml:space="preserve"> new Room('Guidance', 90, 57, 12, 12,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Guidance', 90, 57, 12, 12,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>107</v>
       </c>
@@ -5176,40 +5210,40 @@
       <c r="G41" t="s">
         <v>166</v>
       </c>
-      <c r="H41" t="str">
-        <f>CONCATENATE(" new Room('", A41,"', ", B41,", ", C41,", ",D41,", ",E41, ",[",F41,"],'",G41,"'),")</f>
-        <v xml:space="preserve"> new Room('Special Services', 90, 69, 10, 10,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Special Services', 90, 69, 10, 10,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B42">
         <f>B40+D40</f>
         <v>102</v>
       </c>
       <c r="C42">
-        <f>C145</f>
+        <f>C147</f>
         <v>55</v>
       </c>
       <c r="D42">
-        <f>B145 - (B40+D40)</f>
+        <f>B147 - (B40+D40)</f>
         <v>11</v>
       </c>
       <c r="E42">
         <v>2</v>
       </c>
       <c r="G42" t="s">
-        <v>213</v>
-      </c>
-      <c r="H42" t="str">
-        <f>CONCATENATE(" new Room('", A42,"', ", B42,", ", C42,", ",D42,", ",E42, ",[",F42,"],'",G42,"'),")</f>
-        <v xml:space="preserve"> new Room('Outside', 102, 55, 11, 2,[],'Outside,HideWall-23'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="I42" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve"> new Room('Outside', 102, 55, 11, 2,[],'Outside,HideWall-23',''),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>110</v>
       </c>
@@ -5228,12 +5262,13 @@
       <c r="G44" t="s">
         <v>166</v>
       </c>
-      <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Lecture Hall 501', 33, 54, 11, 4,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" t="str">
+        <f t="shared" ref="I44:I46" si="6">CONCATENATE(" new Room('", A44,"', ", B44,", ", C44,", ",D44,", ",E44, ",[",F44,"],'",G44,"','",H44,"'),")</f>
+        <v xml:space="preserve"> new Room('Lecture Hall 501', 33, 54, 11, 4,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>109</v>
       </c>
@@ -5252,12 +5287,13 @@
       <c r="G45" t="s">
         <v>166</v>
       </c>
-      <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Lecture Hall 502', 16, 54, 11, 4,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> new Room('Lecture Hall 502', 16, 54, 11, 4,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>111</v>
       </c>
@@ -5276,12 +5312,12 @@
       <c r="G46" t="s">
         <v>166</v>
       </c>
-      <c r="H46" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Auditorium', 16, 58, 28, 13,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> new Room('Auditorium', 16, 58, 28, 13,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>-13</v>
       </c>
@@ -5289,7 +5325,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>108</v>
       </c>
@@ -5306,18 +5342,18 @@
         <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G48" t="s">
         <v>166</v>
       </c>
-      <c r="H48" t="str">
-        <f>CONCATENATE(" new Room('", A48,"', ", B48,", ", C48,", ",D48,", ",E48, ",[",F48,"],'",G48,"'),")</f>
-        <v xml:space="preserve"> new Room('Auxillary Gym', 66, 43, 26, 10,[1,1,1,26,3,1,3,26],'Normal'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" t="str">
+        <f>CONCATENATE(" new Room('", A48,"', ", B48,", ", C48,", ",D48,", ",E48, ",[",F48,"],'",G48,"','",H48,"'),")</f>
+        <v xml:space="preserve"> new Room('Auxillary Gym', 66, 43, 26, 10,[1,1,1,26,3,1,3,26],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>157</v>
       </c>
@@ -5336,12 +5372,12 @@
       <c r="G50" t="s">
         <v>166</v>
       </c>
-      <c r="H50" t="str">
-        <f>CONCATENATE(" new Room('", A50,"', ", B50,", ", C50,", ",D50,", ",E50, ",[",F50,"],'",G50,"'),")</f>
-        <v xml:space="preserve"> new Room('Courtyard3', 47, 55, 10, 12,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" t="str">
+        <f t="shared" ref="I50:I53" si="7">CONCATENATE(" new Room('", A50,"', ", B50,", ", C50,", ",D50,", ",E50, ",[",F50,"],'",G50,"','",H50,"'),")</f>
+        <v xml:space="preserve"> new Room('Courtyard3', 47, 55, 10, 12,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>87</v>
       </c>
@@ -5363,12 +5399,12 @@
       <c r="G51" t="s">
         <v>166</v>
       </c>
-      <c r="H51" t="str">
-        <f>CONCATENATE(" new Room('", A51,"', ", B51,", ", C51,", ",D51,", ",E51, ",[",F51,"],'",G51,"'),")</f>
-        <v xml:space="preserve"> new Room('126', 57, 55, 12, 4,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> new Room('126', 57, 55, 12, 4,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>88</v>
       </c>
@@ -5390,12 +5426,12 @@
       <c r="G52" t="s">
         <v>166</v>
       </c>
-      <c r="H52" t="str">
-        <f>CONCATENATE(" new Room('", A52,"', ", B52,", ", C52,", ",D52,", ",E52, ",[",F52,"],'",G52,"'),")</f>
-        <v xml:space="preserve"> new Room('124', 57, 59, 12, 4,[2,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> new Room('124', 57, 59, 12, 4,[2,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>89</v>
       </c>
@@ -5417,13 +5453,13 @@
       <c r="G53" t="s">
         <v>166</v>
       </c>
-      <c r="H53" t="str">
-        <f>CONCATENATE(" new Room('", A53,"', ", B53,", ", C53,", ",D53,", ",E53, ",[",F53,"],'",G53,"'),")</f>
-        <v xml:space="preserve"> new Room('122', 57, 63, 12, 4,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve"> new Room('122', 57, 63, 12, 4,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -5440,17 +5476,17 @@
         <v>4</v>
       </c>
       <c r="F55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G55" t="s">
         <v>166</v>
       </c>
-      <c r="H55" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Band Lockers', 1, 67, 6, 4,[1,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I55" t="str">
+        <f t="shared" ref="I55:I63" si="8">CONCATENATE(" new Room('", A55,"', ", B55,", ", C55,", ",D55,", ",E55, ",[",F55,"],'",G55,"','",H55,"'),")</f>
+        <v xml:space="preserve"> new Room('Band Lockers', 1, 67, 6, 4,[1,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
@@ -5467,17 +5503,17 @@
         <v>3</v>
       </c>
       <c r="F56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G56" t="s">
         <v>166</v>
       </c>
-      <c r="H56" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Band Office', 9, 67, 5, 3,[4,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I56" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Band Office', 9, 67, 5, 3,[4,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>96</v>
       </c>
@@ -5494,17 +5530,17 @@
         <v>9</v>
       </c>
       <c r="F57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G57" t="s">
         <v>166</v>
       </c>
-      <c r="H57" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Band Room', 1, 58, 12, 9,[1,1,1,9],'Normal'),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I57" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Band Room', 1, 58, 12, 9,[1,1,1,9],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -5521,41 +5557,17 @@
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G58" t="s">
         <v>166</v>
       </c>
-      <c r="H58" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Choral Room', 25, 77, 15, 6,[1,1,1,14],'Normal'),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B59">
-        <v>47</v>
-      </c>
-      <c r="C59">
-        <v>68</v>
-      </c>
-      <c r="D59">
-        <v>10</v>
-      </c>
-      <c r="E59">
-        <v>10</v>
-      </c>
-      <c r="G59" t="s">
-        <v>166</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Courtyard2', 47, 68, 10, 10,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I58" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Choral Room', 25, 77, 15, 6,[1,1,1,14],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>99</v>
       </c>
@@ -5572,17 +5584,17 @@
         <v>9</v>
       </c>
       <c r="F60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G60" t="s">
         <v>166</v>
       </c>
-      <c r="H60" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Orchestra', 0, 74, 12, 9,[4,6,2,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I60" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Orchestra', 0, 74, 12, 9,[4,6,2,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>95</v>
       </c>
@@ -5599,17 +5611,17 @@
         <v>5</v>
       </c>
       <c r="F61" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G61" t="s">
         <v>166</v>
       </c>
-      <c r="H61" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Piano Room', 1, 53, 10, 5,[2,1,3,8],'Normal'),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I61" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Piano Room', 1, 53, 10, 5,[2,1,3,8],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>101</v>
       </c>
@@ -5626,17 +5638,17 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G62" t="s">
         <v>166</v>
       </c>
-      <c r="H62" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Sm. Ensemble Room', 16, 80, 6, 3,[1,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I62" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Sm. Ensemble Room', 16, 80, 6, 3,[1,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>112</v>
       </c>
@@ -5653,18 +5665,18 @@
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G63" t="s">
         <v>166</v>
       </c>
-      <c r="H63" t="str">
-        <f t="shared" ref="H63:H132" si="1">CONCATENATE(" new Room('", A63,"', ", B63,", ", C63,", ",D63,", ",E63, ",[",F63,"],'",G63,"'),")</f>
-        <v xml:space="preserve"> new Room('Stage', 16, 71, 28, 5,[4,5,3,2,2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I63" t="str">
+        <f t="shared" si="8"/>
+        <v xml:space="preserve"> new Room('Stage', 16, 71, 28, 5,[4,5,3,2,2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>155</v>
       </c>
@@ -5684,12 +5696,12 @@
       <c r="G65" t="s">
         <v>166</v>
       </c>
-      <c r="H65" t="str">
-        <f t="shared" ref="H65:H71" si="2">CONCATENATE(" new Room('", A65,"', ", B65,", ", C65,", ",D65,", ",E65, ",[",F65,"],'",G65,"'),")</f>
-        <v xml:space="preserve"> new Room('Courtyard1', 51, 18, 7, 23,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" t="str">
+        <f t="shared" ref="I65:I71" si="9">CONCATENATE(" new Room('", A65,"', ", B65,", ", C65,", ",D65,", ",E65, ",[",F65,"],'",G65,"','",H65,"'),")</f>
+        <v xml:space="preserve"> new Room('Courtyard1', 51, 18, 7, 23,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>92</v>
       </c>
@@ -5706,17 +5718,17 @@
         <v>3</v>
       </c>
       <c r="F66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G66" t="s">
         <v>166</v>
       </c>
-      <c r="H66" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('District MDF', 58, 18, 8, 3,[1,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I66" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('District MDF', 58, 18, 8, 3,[1,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>162</v>
       </c>
@@ -5733,17 +5745,17 @@
         <v>3</v>
       </c>
       <c r="F67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G67" t="s">
         <v>166</v>
       </c>
-      <c r="H67" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('MDF1', 66, 18, 7, 3,[1,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I67" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('MDF1', 66, 18, 7, 3,[1,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>272</v>
       </c>
@@ -5765,12 +5777,12 @@
       <c r="G68" t="s">
         <v>166</v>
       </c>
-      <c r="H68" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('272', 58, 21, 15, 5,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I68" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('272', 58, 21, 15, 5,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>276</v>
       </c>
@@ -5792,12 +5804,12 @@
       <c r="G69" t="s">
         <v>166</v>
       </c>
-      <c r="H69" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('276', 58, 26, 15, 5,[2,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I69" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('276', 58, 26, 15, 5,[2,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>278</v>
       </c>
@@ -5819,12 +5831,12 @@
       <c r="G70" t="s">
         <v>166</v>
       </c>
-      <c r="H70" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('278', 58, 31, 15, 5,[2,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I70" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('278', 58, 31, 15, 5,[2,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>282</v>
       </c>
@@ -5846,213 +5858,261 @@
       <c r="G71" t="s">
         <v>166</v>
       </c>
-      <c r="H71" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve"> new Room('282', 58, 36, 15, 5,[2,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="I71" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve"> new Room('282', 58, 36, 15, 5,[2,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73">
+        <v>47</v>
+      </c>
+      <c r="C73">
+        <v>68</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73">
+        <v>10</v>
+      </c>
+      <c r="G73" t="s">
+        <v>166</v>
+      </c>
+      <c r="I73" t="str">
+        <f>CONCATENATE(" new Room('", A73,"', ", B73,", ", C73,", ",D73,", ",E73, ",[",F73,"],'",G73,"','",H73,"'),")</f>
+        <v xml:space="preserve"> new Room('Courtyard2', 47, 68, 10, 10,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74">
+        <f>B73+D73</f>
+        <v>57</v>
+      </c>
+      <c r="C74">
+        <v>68</v>
+      </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>5</v>
+      </c>
+      <c r="G74" t="s">
+        <v>166</v>
+      </c>
+      <c r="I74" t="str">
+        <f>CONCATENATE(" new Room('", A74,"', ", B74,", ", C74,", ",D74,", ",E74, ",[",F74,"],'",G74,"','",H74,"'),")</f>
+        <v xml:space="preserve"> new Room('120', 57, 68, 12, 5,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B75">
+        <f>B73+D73</f>
+        <v>57</v>
+      </c>
+      <c r="C75">
+        <f>C74+E74</f>
+        <v>73</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75">
+        <v>5</v>
+      </c>
+      <c r="G75" t="s">
+        <v>166</v>
+      </c>
+      <c r="I75" t="str">
+        <f>CONCATENATE(" new Room('", A75,"', ", B75,", ", C75,", ",D75,", ",E75, ",[",F75,"],'",G75,"','",H75,"'),")</f>
+        <v xml:space="preserve"> new Room('Nurse', 57, 73, 12, 5,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B76">
+        <v>49</v>
+      </c>
+      <c r="C76">
+        <f>C75+E75</f>
+        <v>78</v>
+      </c>
+      <c r="D76">
+        <f>C75+E75-B76</f>
+        <v>29</v>
+      </c>
+      <c r="E76">
+        <v>4</v>
+      </c>
+      <c r="G76" t="s">
+        <v>166</v>
+      </c>
+      <c r="H76" t="s">
+        <v>102</v>
+      </c>
+      <c r="I76" t="str">
+        <f>CONCATENATE(" new Room('", A76,"', ", B76,", ", C76,", ",D76,", ",E76, ",[",F76,"],'",G76,"','",H76,"'),")</f>
+        <v xml:space="preserve"> new Room('Admin Office', 49, 78, 29, 4,[],'Normal','Main Office'),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>242</v>
       </c>
-      <c r="B76">
+      <c r="B78">
         <v>84</v>
       </c>
-      <c r="C76">
+      <c r="C78">
         <v>19</v>
       </c>
-      <c r="D76">
+      <c r="D78">
         <v>17</v>
       </c>
-      <c r="E76">
+      <c r="E78">
         <v>9</v>
       </c>
-      <c r="F76" t="s">
-        <v>197</v>
-      </c>
-      <c r="G76" t="s">
-        <v>166</v>
-      </c>
-      <c r="H76" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('242', 84, 19, 17, 9,[1,14,2,8],'Normal'),</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="F78" t="s">
+        <v>196</v>
+      </c>
+      <c r="G78" t="s">
+        <v>166</v>
+      </c>
+      <c r="I78" t="str">
+        <f>CONCATENATE(" new Room('", A78,"', ", B78,", ", C78,", ",D78,", ",E78, ",[",F78,"],'",G78,"','",H78,"'),")</f>
+        <v xml:space="preserve"> new Room('242', 84, 19, 17, 9,[1,14,2,8],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
         <v>263</v>
       </c>
-      <c r="B79">
+      <c r="B81">
         <v>84</v>
       </c>
-      <c r="C79">
+      <c r="C81">
         <v>19</v>
       </c>
-      <c r="D79">
+      <c r="D81">
         <v>8</v>
       </c>
-      <c r="E79">
+      <c r="E81">
         <v>5</v>
       </c>
-      <c r="F79" t="s">
-        <v>194</v>
-      </c>
-      <c r="G79" t="s">
-        <v>166</v>
-      </c>
-      <c r="H79" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('263', 84, 19, 8, 5,[1,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="F81" t="s">
+        <v>193</v>
+      </c>
+      <c r="G81" t="s">
+        <v>166</v>
+      </c>
+      <c r="I81" t="str">
+        <f t="shared" ref="I81:I89" si="10">CONCATENATE(" new Room('", A81,"', ", B81,", ", C81,", ",D81,", ",E81, ",[",F81,"],'",G81,"','",H81,"'),")</f>
+        <v xml:space="preserve"> new Room('263', 84, 19, 8, 5,[1,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
         <v>265</v>
-      </c>
-      <c r="B80">
-        <v>75</v>
-      </c>
-      <c r="C80">
-        <v>19</v>
-      </c>
-      <c r="D80">
-        <v>9</v>
-      </c>
-      <c r="E80">
-        <v>3</v>
-      </c>
-      <c r="F80" t="s">
-        <v>198</v>
-      </c>
-      <c r="G80" t="s">
-        <v>166</v>
-      </c>
-      <c r="H80" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('265', 75, 19, 9, 3,[1,9],'Normal'),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>266</v>
-      </c>
-      <c r="B81">
-        <v>75</v>
-      </c>
-      <c r="C81">
-        <v>22</v>
-      </c>
-      <c r="D81">
-        <v>9</v>
-      </c>
-      <c r="E81">
-        <v>4</v>
-      </c>
-      <c r="F81" t="s">
-        <v>199</v>
-      </c>
-      <c r="G81" t="s">
-        <v>166</v>
-      </c>
-      <c r="H81" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('266', 75, 22, 9, 4,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
-        <v>267</v>
       </c>
       <c r="B82">
         <v>75</v>
       </c>
       <c r="C82">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D82">
         <v>9</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F82" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G82" t="s">
         <v>166</v>
       </c>
-      <c r="H82" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('267', 75, 26, 9, 5,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I82" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('265', 75, 19, 9, 3,[1,9],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B83">
         <v>75</v>
       </c>
       <c r="C83">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D83">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E83">
         <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G83" t="s">
         <v>166</v>
       </c>
-      <c r="H83" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('275', 75, 31, 12, 4,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I83" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('266', 75, 22, 9, 4,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="B84">
         <v>75</v>
       </c>
       <c r="C84">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D84">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E84">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="G84" t="s">
         <v>166</v>
       </c>
-      <c r="H84" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('281', 75, 37, 12, 4,[4,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I84" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('267', 75, 26, 9, 5,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B85">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C85">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D85">
         <v>12</v>
@@ -6061,25 +6121,25 @@
         <v>4</v>
       </c>
       <c r="F85" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="G85" t="s">
         <v>166</v>
       </c>
-      <c r="H85" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('283', 87, 37, 12, 4,[3,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I85" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('275', 75, 31, 12, 4,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="B86">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C86">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D86">
         <v>12</v>
@@ -6088,132 +6148,102 @@
         <v>4</v>
       </c>
       <c r="F86" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="G86" t="s">
         <v>166</v>
       </c>
-      <c r="H86" t="str">
-        <f>CONCATENATE(" new Room('", A86,"', ", B86,", ", C86,", ",D86,", ",E86, ",[",F86,"],'",G86,"'),")</f>
-        <v xml:space="preserve"> new Room('248', 87, 33, 12, 4,[2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="I86" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('281', 75, 37, 12, 4,[4,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>283</v>
+      </c>
+      <c r="B87">
+        <v>87</v>
+      </c>
+      <c r="C87">
+        <v>37</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87">
+        <v>4</v>
+      </c>
+      <c r="F87" t="s">
+        <v>178</v>
+      </c>
+      <c r="G87" t="s">
+        <v>166</v>
+      </c>
+      <c r="I87" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('283', 87, 37, 12, 4,[3,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>248</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <v>33</v>
+      </c>
+      <c r="D88">
+        <v>12</v>
+      </c>
+      <c r="E88">
+        <v>4</v>
+      </c>
+      <c r="F88" t="s">
+        <v>199</v>
+      </c>
+      <c r="G88" t="s">
+        <v>166</v>
+      </c>
+      <c r="I88" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('248', 87, 33, 12, 4,[2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B87">
+      <c r="B89">
         <v>84</v>
       </c>
-      <c r="C87">
+      <c r="C89">
         <v>28</v>
       </c>
-      <c r="D87">
+      <c r="D89">
         <v>9</v>
       </c>
-      <c r="E87">
+      <c r="E89">
         <v>3</v>
       </c>
-      <c r="G87" t="s">
-        <v>166</v>
-      </c>
-      <c r="H87" t="str">
-        <f>CONCATENATE(" new Room('", A87,"', ", B87,", ", C87,", ",D87,", ",E87, ",[",F87,"],'",G87,"'),")</f>
-        <v xml:space="preserve"> new Room('mech4', 84, 28, 9, 3,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89">
-        <v>58</v>
-      </c>
-      <c r="C89">
-        <v>69</v>
-      </c>
-      <c r="D89">
-        <v>11</v>
-      </c>
-      <c r="E89">
-        <v>6</v>
-      </c>
       <c r="G89" t="s">
         <v>166</v>
       </c>
-      <c r="H89" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('120', 58, 69, 11, 6,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="I89" t="str">
+        <f t="shared" si="10"/>
+        <v xml:space="preserve"> new Room('mech4', 84, 28, 9, 3,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B91">
+      <c r="B93">
         <v>75</v>
-      </c>
-      <c r="C91">
-        <v>6</v>
-      </c>
-      <c r="D91">
-        <v>7</v>
-      </c>
-      <c r="E91">
-        <v>5</v>
-      </c>
-      <c r="F91" t="s">
-        <v>201</v>
-      </c>
-      <c r="G91" t="s">
-        <v>166</v>
-      </c>
-      <c r="H91" t="str">
-        <f t="shared" ref="H91:H99" si="3">CONCATENATE(" new Room('", A91,"', ", B91,", ", C91,", ",D91,", ",E91, ",[",F91,"],'",G91,"'),")</f>
-        <v xml:space="preserve"> new Room('251', 75, 6, 7, 5,[1,7],'Normal'),</v>
-      </c>
-      <c r="J91">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B92">
-        <v>82</v>
-      </c>
-      <c r="C92">
-        <v>6</v>
-      </c>
-      <c r="D92">
-        <v>8</v>
-      </c>
-      <c r="E92">
-        <v>5</v>
-      </c>
-      <c r="F92" t="s">
-        <v>202</v>
-      </c>
-      <c r="G92" t="s">
-        <v>166</v>
-      </c>
-      <c r="H92" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('252', 82, 6, 8, 5,[1,8],'Normal'),</v>
-      </c>
-      <c r="J92">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B93">
-        <v>90</v>
       </c>
       <c r="C93">
         <v>6</v>
@@ -6222,58 +6252,61 @@
         <v>7</v>
       </c>
       <c r="E93">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F93" t="s">
+        <v>200</v>
+      </c>
+      <c r="G93" t="s">
+        <v>166</v>
+      </c>
+      <c r="I93" t="str">
+        <f t="shared" ref="I93:I101" si="11">CONCATENATE(" new Room('", A93,"', ", B93,", ", C93,", ",D93,", ",E93, ",[",F93,"],'",G93,"','",H93,"'),")</f>
+        <v xml:space="preserve"> new Room('251', 75, 6, 7, 5,[1,7],'Normal',''),</v>
+      </c>
+      <c r="K93">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B94">
+        <v>82</v>
+      </c>
+      <c r="C94">
+        <v>6</v>
+      </c>
+      <c r="D94">
+        <v>8</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+      <c r="F94" t="s">
         <v>201</v>
       </c>
-      <c r="G93" t="s">
-        <v>166</v>
-      </c>
-      <c r="H93" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('255', 90, 6, 7, 4,[1,7],'Normal'),</v>
-      </c>
-      <c r="J93" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
-        <v>253</v>
-      </c>
-      <c r="B94">
-        <v>90</v>
-      </c>
-      <c r="C94">
-        <v>10</v>
-      </c>
-      <c r="D94">
-        <v>7</v>
-      </c>
-      <c r="E94">
-        <v>4</v>
-      </c>
-      <c r="F94" t="s">
-        <v>177</v>
-      </c>
       <c r="G94" t="s">
         <v>166</v>
       </c>
-      <c r="H94" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('253', 90, 10, 7, 4,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
-        <v>260</v>
+      <c r="I94" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('252', 82, 6, 8, 5,[1,8],'Normal',''),</v>
+      </c>
+      <c r="K94">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B95">
         <v>90</v>
       </c>
       <c r="C95">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D95">
         <v>7</v>
@@ -6282,25 +6315,28 @@
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="G95" t="s">
         <v>166</v>
       </c>
-      <c r="H95" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('260', 90, 14, 7, 4,[3,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I95" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('255', 90, 6, 7, 4,[1,7],'Normal',''),</v>
+      </c>
+      <c r="K95" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B96">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C96">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D96">
         <v>7</v>
@@ -6309,370 +6345,370 @@
         <v>4</v>
       </c>
       <c r="F96" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G96" t="s">
         <v>166</v>
       </c>
-      <c r="H96" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('262', 83, 14, 7, 4,[3,7],'Normal'),</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I96" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('253', 90, 10, 7, 4,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B97">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C97">
         <v>14</v>
       </c>
       <c r="D97">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E97">
         <v>4</v>
       </c>
       <c r="F97" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="G97" t="s">
         <v>166</v>
       </c>
-      <c r="H97" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('264', 75, 14, 8, 4,[3,8],'Normal'),</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I97" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('260', 90, 14, 7, 4,[3,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
+        <v>262</v>
+      </c>
+      <c r="B98">
+        <v>83</v>
+      </c>
+      <c r="C98">
+        <v>14</v>
+      </c>
+      <c r="D98">
+        <v>7</v>
+      </c>
+      <c r="E98">
+        <v>4</v>
+      </c>
+      <c r="F98" t="s">
+        <v>187</v>
+      </c>
+      <c r="G98" t="s">
+        <v>166</v>
+      </c>
+      <c r="I98" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('262', 83, 14, 7, 4,[3,7],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>264</v>
+      </c>
+      <c r="B99">
+        <v>75</v>
+      </c>
+      <c r="C99">
+        <v>14</v>
+      </c>
+      <c r="D99">
+        <v>8</v>
+      </c>
+      <c r="E99">
+        <v>4</v>
+      </c>
+      <c r="F99" t="s">
+        <v>202</v>
+      </c>
+      <c r="G99" t="s">
+        <v>166</v>
+      </c>
+      <c r="I99" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('264', 75, 14, 8, 4,[3,8],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
         <v>288</v>
       </c>
-      <c r="B98">
+      <c r="B100">
         <v>75</v>
       </c>
-      <c r="C98">
+      <c r="C100">
         <v>11</v>
       </c>
-      <c r="D98">
+      <c r="D100">
         <v>15</v>
       </c>
-      <c r="E98">
+      <c r="E100">
         <v>3</v>
       </c>
-      <c r="F98" t="s">
-        <v>186</v>
-      </c>
-      <c r="G98" t="s">
-        <v>166</v>
-      </c>
-      <c r="H98" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('288', 75, 11, 15, 3,[4,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="F100" t="s">
+        <v>185</v>
+      </c>
+      <c r="G100" t="s">
+        <v>166</v>
+      </c>
+      <c r="I100" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('288', 75, 11, 15, 3,[4,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B99">
+      <c r="B101">
         <v>97</v>
       </c>
-      <c r="C99">
+      <c r="C101">
         <v>15</v>
       </c>
-      <c r="D99">
+      <c r="D101">
         <v>3</v>
-      </c>
-      <c r="E99">
-        <v>3</v>
-      </c>
-      <c r="F99" t="s">
-        <v>194</v>
-      </c>
-      <c r="G99" t="s">
-        <v>166</v>
-      </c>
-      <c r="H99" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve"> new Room('MDF2', 97, 15, 3, 3,[1,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B101">
-        <v>121</v>
-      </c>
-      <c r="C101">
-        <v>14</v>
-      </c>
-      <c r="D101">
-        <f>D102</f>
-        <v>8</v>
       </c>
       <c r="E101">
         <v>3</v>
       </c>
       <c r="F101" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="G101" t="s">
         <v>166</v>
       </c>
-      <c r="H101" t="str">
-        <f t="shared" ref="H101:H111" si="4">CONCATENATE(" new Room('", A101,"', ", B101,", ", C101,", ",D101,", ",E101, ",[",F101,"],'",G101,"'),")</f>
-        <v xml:space="preserve"> new Room('204', 121, 14, 8, 3,[2,1,2,2],'Normal'),</v>
-      </c>
-      <c r="J101">
+      <c r="I101" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> new Room('MDF2', 97, 15, 3, 3,[1,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B103">
+        <v>121</v>
+      </c>
+      <c r="C103">
+        <v>14</v>
+      </c>
+      <c r="D103">
+        <f>D104</f>
+        <v>8</v>
+      </c>
+      <c r="E103">
+        <v>3</v>
+      </c>
+      <c r="F103" t="s">
+        <v>203</v>
+      </c>
+      <c r="G103" t="s">
+        <v>166</v>
+      </c>
+      <c r="I103" t="str">
+        <f t="shared" ref="I103:I113" si="12">CONCATENATE(" new Room('", A103,"', ", B103,", ", C103,", ",D103,", ",E103, ",[",F103,"],'",G103,"','",H103,"'),")</f>
+        <v xml:space="preserve"> new Room('204', 121, 14, 8, 3,[2,1,2,2],'Normal',''),</v>
+      </c>
+      <c r="K103">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="104" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B102">
-        <v>121</v>
-      </c>
-      <c r="C102">
-        <v>11</v>
-      </c>
-      <c r="D102">
-        <v>8</v>
-      </c>
-      <c r="E102">
-        <v>3</v>
-      </c>
-      <c r="F102" t="s">
-        <v>200</v>
-      </c>
-      <c r="G102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H102" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('205', 121, 11, 8, 3,[2,1],'Normal'),</v>
-      </c>
-      <c r="J102">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B103">
-        <v>101</v>
-      </c>
-      <c r="C103">
-        <v>10</v>
-      </c>
-      <c r="D103">
-        <f>D108+D109+D110+D111</f>
-        <v>20</v>
-      </c>
-      <c r="E103">
-        <f>E102</f>
-        <v>3</v>
-      </c>
-      <c r="G103" t="s">
-        <v>166</v>
-      </c>
-      <c r="H103" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('Courtyard6', 101, 10, 20, 3,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="B104">
         <v>121</v>
       </c>
       <c r="C104">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D104">
-        <f>D102</f>
         <v>8</v>
       </c>
       <c r="E104">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F104" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="G104" t="s">
         <v>166</v>
       </c>
-      <c r="H104" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('206', 121, 6, 8, 5,[2,1,1,3],'Normal'),</v>
-      </c>
-      <c r="J104">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I104" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('205', 121, 11, 8, 3,[2,1],'Normal',''),</v>
+      </c>
+      <c r="K104">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>52</v>
+        <v>160</v>
       </c>
       <c r="B105">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C105">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D105">
-        <v>5</v>
+        <f>D110+D111+D112+D113</f>
+        <v>20</v>
       </c>
       <c r="E105">
-        <v>4</v>
-      </c>
-      <c r="F105" t="s">
-        <v>189</v>
+        <f>E104</f>
+        <v>3</v>
       </c>
       <c r="G105" t="s">
         <v>166</v>
       </c>
-      <c r="H105" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('207', 116, 6, 5, 4,[1,4],'Normal'),</v>
-      </c>
-      <c r="J105">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I105" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('Courtyard6', 101, 10, 20, 3,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B106">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C106">
         <v>6</v>
       </c>
       <c r="D106">
+        <f>D104</f>
+        <v>8</v>
+      </c>
+      <c r="E106">
+        <v>5</v>
+      </c>
+      <c r="F106" t="s">
+        <v>204</v>
+      </c>
+      <c r="G106" t="s">
+        <v>166</v>
+      </c>
+      <c r="I106" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('206', 121, 6, 8, 5,[2,1,1,3],'Normal',''),</v>
+      </c>
+      <c r="K106">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B107">
+        <v>116</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="D107">
+        <v>5</v>
+      </c>
+      <c r="E107">
+        <v>4</v>
+      </c>
+      <c r="F107" t="s">
+        <v>188</v>
+      </c>
+      <c r="G107" t="s">
+        <v>166</v>
+      </c>
+      <c r="I107" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('207', 116, 6, 5, 4,[1,4],'Normal',''),</v>
+      </c>
+      <c r="K107">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B108">
+        <v>108</v>
+      </c>
+      <c r="C108">
+        <v>6</v>
+      </c>
+      <c r="D108">
         <f>D31</f>
         <v>8</v>
       </c>
-      <c r="E106">
-        <f>E107</f>
+      <c r="E108">
+        <f>E109</f>
         <v>4</v>
       </c>
-      <c r="F106" t="s">
-        <v>196</v>
-      </c>
-      <c r="G106" t="s">
-        <v>166</v>
-      </c>
-      <c r="H106" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('208', 108, 6, 8, 4,[1,2],'Normal'),</v>
-      </c>
-      <c r="J106">
+      <c r="F108" t="s">
+        <v>195</v>
+      </c>
+      <c r="G108" t="s">
+        <v>166</v>
+      </c>
+      <c r="I108" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('208', 108, 6, 8, 4,[1,2],'Normal',''),</v>
+      </c>
+      <c r="K108">
         <v>143</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="109" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B107">
+      <c r="B109">
         <v>100</v>
       </c>
-      <c r="C107">
+      <c r="C109">
         <v>6</v>
       </c>
-      <c r="D107">
+      <c r="D109">
         <f>D30</f>
         <v>8</v>
       </c>
-      <c r="E107">
-        <f>E93</f>
+      <c r="E109">
+        <f>E95</f>
         <v>4</v>
       </c>
-      <c r="F107" t="s">
-        <v>207</v>
-      </c>
-      <c r="G107" t="s">
-        <v>166</v>
-      </c>
-      <c r="H107" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('209', 100, 6, 8, 4,[1,5],'Normal'),</v>
-      </c>
-      <c r="J107">
+      <c r="F109" t="s">
+        <v>206</v>
+      </c>
+      <c r="G109" t="s">
+        <v>166</v>
+      </c>
+      <c r="I109" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('209', 100, 6, 8, 4,[1,5],'Normal',''),</v>
+      </c>
+      <c r="K109">
         <v>145</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
+    <row r="110" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B108">
+      <c r="B110">
         <v>101</v>
-      </c>
-      <c r="C108">
-        <v>13</v>
-      </c>
-      <c r="D108">
-        <v>5</v>
-      </c>
-      <c r="E108">
-        <v>4</v>
-      </c>
-      <c r="F108" t="s">
-        <v>206</v>
-      </c>
-      <c r="G108" t="s">
-        <v>166</v>
-      </c>
-      <c r="H108" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('200', 101, 13, 5, 4,[3,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B109">
-        <v>106</v>
-      </c>
-      <c r="C109">
-        <v>13</v>
-      </c>
-      <c r="D109">
-        <v>5</v>
-      </c>
-      <c r="E109">
-        <v>4</v>
-      </c>
-      <c r="F109" t="s">
-        <v>178</v>
-      </c>
-      <c r="G109" t="s">
-        <v>166</v>
-      </c>
-      <c r="H109" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('201', 106, 13, 5, 4,[3,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B110">
-        <v>111</v>
       </c>
       <c r="C110">
         <v>13</v>
@@ -6684,22 +6720,22 @@
         <v>4</v>
       </c>
       <c r="F110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G110" t="s">
         <v>166</v>
       </c>
-      <c r="H110" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('202', 111, 13, 5, 4,[3,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I110" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('200', 101, 13, 5, 4,[3,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B111">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C111">
         <v>13</v>
@@ -6716,298 +6752,295 @@
       <c r="G111" t="s">
         <v>166</v>
       </c>
-      <c r="H111" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> new Room('203', 116, 13, 5, 4,[3,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I111" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('201', 106, 13, 5, 4,[3,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112">
+        <v>13</v>
+      </c>
+      <c r="D112">
+        <v>5</v>
+      </c>
+      <c r="E112">
+        <v>4</v>
+      </c>
+      <c r="F112" t="s">
+        <v>205</v>
+      </c>
+      <c r="G112" t="s">
+        <v>166</v>
+      </c>
+      <c r="I112" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('202', 111, 13, 5, 4,[3,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113">
+        <v>116</v>
+      </c>
+      <c r="C113">
+        <v>13</v>
+      </c>
+      <c r="D113">
+        <v>5</v>
+      </c>
+      <c r="E113">
+        <v>4</v>
+      </c>
+      <c r="F113" t="s">
+        <v>178</v>
+      </c>
+      <c r="G113" t="s">
+        <v>166</v>
+      </c>
+      <c r="I113" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> new Room('203', 116, 13, 5, 4,[3,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B113">
+      <c r="B115">
         <v>134</v>
       </c>
-      <c r="C113">
+      <c r="C115">
         <v>7</v>
       </c>
-      <c r="D113">
+      <c r="D115">
         <v>9</v>
       </c>
-      <c r="E113">
+      <c r="E115">
         <v>11</v>
       </c>
-      <c r="F113" t="s">
-        <v>208</v>
-      </c>
-      <c r="G113" t="s">
-        <v>166</v>
-      </c>
-      <c r="H113" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('221', 134, 7, 9, 11,[4,6],'Normal'),</v>
-      </c>
-      <c r="J113">
+      <c r="F115" t="s">
+        <v>207</v>
+      </c>
+      <c r="G115" t="s">
+        <v>166</v>
+      </c>
+      <c r="I115" t="str">
+        <f t="shared" ref="I115:I122" si="13">CONCATENATE(" new Room('", A115,"', ", B115,", ", C115,", ",D115,", ",E115, ",[",F115,"],'",G115,"','",H115,"'),")</f>
+        <v xml:space="preserve"> new Room('221', 134, 7, 9, 11,[4,6],'Normal',''),</v>
+      </c>
+      <c r="K115">
         <v>136</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+    <row r="116" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B114">
-        <v>117</v>
-      </c>
-      <c r="C114">
-        <v>19</v>
-      </c>
-      <c r="D114">
-        <v>5</v>
-      </c>
-      <c r="E114">
-        <v>3</v>
-      </c>
-      <c r="F114" t="s">
-        <v>176</v>
-      </c>
-      <c r="G114" t="s">
-        <v>166</v>
-      </c>
-      <c r="H114" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('226', 117, 19, 5, 3,[2,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B115">
-        <v>117</v>
-      </c>
-      <c r="C115">
-        <v>22</v>
-      </c>
-      <c r="D115">
-        <f>D114</f>
-        <v>5</v>
-      </c>
-      <c r="E115">
-        <f>E114</f>
-        <v>3</v>
-      </c>
-      <c r="F115" t="s">
-        <v>176</v>
-      </c>
-      <c r="G115" t="s">
-        <v>166</v>
-      </c>
-      <c r="H115" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('228', 117, 22, 5, 3,[2,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="B116">
         <v>117</v>
       </c>
       <c r="C116">
+        <v>19</v>
+      </c>
+      <c r="D116">
+        <v>5</v>
+      </c>
+      <c r="E116">
+        <v>3</v>
+      </c>
+      <c r="F116" t="s">
+        <v>176</v>
+      </c>
+      <c r="G116" t="s">
+        <v>166</v>
+      </c>
+      <c r="I116" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('226', 117, 19, 5, 3,[2,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B117">
+        <v>117</v>
+      </c>
+      <c r="C117">
+        <v>22</v>
+      </c>
+      <c r="D117">
+        <f>D116</f>
+        <v>5</v>
+      </c>
+      <c r="E117">
+        <f>E116</f>
+        <v>3</v>
+      </c>
+      <c r="F117" t="s">
+        <v>176</v>
+      </c>
+      <c r="G117" t="s">
+        <v>166</v>
+      </c>
+      <c r="I117" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('228', 117, 22, 5, 3,[2,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118">
         <v>25</v>
       </c>
-      <c r="D116">
-        <f>D115</f>
+      <c r="D118">
+        <f>D117</f>
         <v>5</v>
       </c>
-      <c r="E116">
-        <f>E115</f>
+      <c r="E118">
+        <f>E117</f>
         <v>3</v>
       </c>
-      <c r="F116" t="s">
-        <v>200</v>
-      </c>
-      <c r="G116" t="s">
-        <v>166</v>
-      </c>
-      <c r="H116" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('230', 117, 25, 5, 3,[2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="F118" t="s">
+        <v>199</v>
+      </c>
+      <c r="G118" t="s">
+        <v>166</v>
+      </c>
+      <c r="I118" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('230', 117, 25, 5, 3,[2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B117">
-        <v>109</v>
-      </c>
-      <c r="C117">
-        <v>30</v>
-      </c>
-      <c r="D117">
-        <v>6</v>
-      </c>
-      <c r="E117">
-        <v>3</v>
-      </c>
-      <c r="G117" t="s">
-        <v>166</v>
-      </c>
-      <c r="H117" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('232', 109, 30, 6, 3,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B118">
-        <v>114</v>
-      </c>
-      <c r="C118">
-        <v>28</v>
-      </c>
-      <c r="D118">
-        <v>8</v>
-      </c>
-      <c r="E118">
-        <v>5</v>
-      </c>
-      <c r="G118" t="s">
-        <v>166</v>
-      </c>
-      <c r="H118" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('234', 114, 28, 8, 5,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="B119">
         <v>109</v>
       </c>
       <c r="C119">
+        <v>30</v>
+      </c>
+      <c r="D119">
+        <v>6</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+      <c r="G119" t="s">
+        <v>166</v>
+      </c>
+      <c r="I119" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('232', 109, 30, 6, 3,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B120">
+        <v>114</v>
+      </c>
+      <c r="C120">
         <v>28</v>
       </c>
-      <c r="D119">
+      <c r="D120">
+        <v>8</v>
+      </c>
+      <c r="E120">
         <v>5</v>
       </c>
-      <c r="E119">
+      <c r="G120" t="s">
+        <v>166</v>
+      </c>
+      <c r="I120" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('234', 114, 28, 8, 5,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B121">
+        <v>109</v>
+      </c>
+      <c r="C121">
+        <v>28</v>
+      </c>
+      <c r="D121">
+        <v>5</v>
+      </c>
+      <c r="E121">
         <v>2</v>
       </c>
-      <c r="G119" t="s">
-        <v>166</v>
-      </c>
-      <c r="H119" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('235', 109, 28, 5, 2,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="G121" t="s">
+        <v>166</v>
+      </c>
+      <c r="I121" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('235', 109, 28, 5, 2,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B120">
+      <c r="B122">
         <v>103</v>
       </c>
-      <c r="C120">
+      <c r="C122">
         <v>19</v>
       </c>
-      <c r="D120">
+      <c r="D122">
         <v>14</v>
       </c>
-      <c r="E120">
-        <f>E114+E115+E116</f>
+      <c r="E122">
+        <f>E116+E117+E118</f>
         <v>9</v>
       </c>
-      <c r="F120" t="s">
-        <v>196</v>
-      </c>
-      <c r="G120" t="s">
-        <v>166</v>
-      </c>
-      <c r="H120" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('240/241', 103, 19, 14, 9,[1,2],'Normal'),</v>
-      </c>
-      <c r="J120">
+      <c r="F122" t="s">
+        <v>195</v>
+      </c>
+      <c r="G122" t="s">
+        <v>166</v>
+      </c>
+      <c r="I122" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> new Room('240/241', 103, 19, 14, 9,[1,2],'Normal',''),</v>
+      </c>
+      <c r="K122">
         <v>154</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+    <row r="123" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B123">
-        <v>125</v>
-      </c>
-      <c r="C123">
-        <v>18</v>
-      </c>
-      <c r="D123">
-        <v>18</v>
-      </c>
-      <c r="E123">
-        <v>5</v>
-      </c>
-      <c r="F123" t="s">
-        <v>187</v>
-      </c>
-      <c r="G123" t="s">
-        <v>166</v>
-      </c>
-      <c r="H123" t="str">
-        <f>CONCATENATE(" new Room('", A123,"', ", B123,", ", C123,", ",D123,", ",E123, ",[",F123,"],'",G123,"'),")</f>
-        <v xml:space="preserve"> new Room('225', 125, 18, 18, 5,[4,3],'Normal'),</v>
-      </c>
-      <c r="J123">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B124">
-        <v>125</v>
-      </c>
-      <c r="C124">
-        <v>23</v>
-      </c>
-      <c r="D124">
-        <v>18</v>
-      </c>
-      <c r="E124">
-        <v>5</v>
-      </c>
-      <c r="F124" t="s">
-        <v>186</v>
-      </c>
-      <c r="G124" t="s">
-        <v>166</v>
-      </c>
-      <c r="H124" t="str">
-        <f t="shared" ref="H124:H125" si="5">CONCATENATE(" new Room('", A124,"', ", B124,", ", C124,", ",D124,", ",E124, ",[",F124,"],'",G124,"'),")</f>
-        <v xml:space="preserve"> new Room('229', 125, 23, 18, 5,[4,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>171</v>
       </c>
       <c r="B125">
         <v>125</v>
       </c>
       <c r="C125">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D125">
         <v>18</v>
@@ -7016,133 +7049,136 @@
         <v>5</v>
       </c>
       <c r="F125" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="G125" t="s">
         <v>166</v>
       </c>
-      <c r="H125" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> new Room('231', 125, 28, 18, 5,[4,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I125" t="str">
+        <f t="shared" ref="I125:I136" si="14">CONCATENATE(" new Room('", A125,"', ", B125,", ", C125,", ",D125,", ",E125, ",[",F125,"],'",G125,"','",H125,"'),")</f>
+        <v xml:space="preserve"> new Room('225', 125, 18, 18, 5,[4,3],'Normal',''),</v>
+      </c>
+      <c r="K125">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B126">
         <v>125</v>
       </c>
       <c r="C126">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D126">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E126">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F126" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="G126" t="s">
-        <v>214</v>
-      </c>
-      <c r="H126" t="str">
-        <f>CONCATENATE(" new Room('", A126,"', ", B126,", ", C126,", ",D126,", ",E126, ",[",F126,"],'",G126,"'),")</f>
-        <v xml:space="preserve"> new Room('stairs1', 125, 33, 10, 2,[4,1,4,2],'Stair'),</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="I126" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('229', 125, 23, 18, 5,[4,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>80</v>
+        <v>171</v>
       </c>
       <c r="B127">
         <v>125</v>
       </c>
       <c r="C127">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D127">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E127">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F127" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G127" t="s">
         <v>166</v>
       </c>
-      <c r="H127" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('305', 125, 35, 10, 4,[4,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I127" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('231', 125, 28, 18, 5,[4,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="B128">
         <v>125</v>
       </c>
       <c r="C128">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D128">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E128">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F128" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
       <c r="G128" t="s">
-        <v>166</v>
-      </c>
-      <c r="H128" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('311', 125, 39, 9, 4,[4,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="I128" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('stairs1', 125, 33, 10, 2,[4,1,4,2],'Stair',''),</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B129">
         <v>125</v>
       </c>
       <c r="C129">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D129">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E129">
         <v>4</v>
       </c>
       <c r="F129" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="G129" t="s">
         <v>166</v>
       </c>
-      <c r="H129" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('313', 125, 43, 9, 4,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I129" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('305', 125, 35, 10, 4,[4,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B130">
         <v>125</v>
       </c>
       <c r="C130">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D130">
         <v>9</v>
@@ -7151,25 +7187,25 @@
         <v>4</v>
       </c>
       <c r="F130" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G130" t="s">
         <v>166</v>
       </c>
-      <c r="H130" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('315', 125, 47, 9, 4,[4,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I130" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('311', 125, 39, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B131">
         <v>125</v>
       </c>
       <c r="C131">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D131">
         <v>9</v>
@@ -7178,25 +7214,25 @@
         <v>4</v>
       </c>
       <c r="F131" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G131" t="s">
         <v>166</v>
       </c>
-      <c r="H131" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('317', 125, 51, 9, 4,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I131" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('313', 125, 43, 9, 4,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B132">
         <v>125</v>
       </c>
       <c r="C132">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D132">
         <v>9</v>
@@ -7205,25 +7241,25 @@
         <v>4</v>
       </c>
       <c r="F132" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G132" t="s">
         <v>166</v>
       </c>
-      <c r="H132" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> new Room('319', 125, 55, 9, 4,[4,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I132" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('315', 125, 47, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B133">
         <v>125</v>
       </c>
       <c r="C133">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D133">
         <v>9</v>
@@ -7232,266 +7268,266 @@
         <v>4</v>
       </c>
       <c r="F133" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G133" t="s">
         <v>166</v>
       </c>
-      <c r="H133" t="str">
-        <f t="shared" ref="H133:H147" si="6">CONCATENATE(" new Room('", A133,"', ", B133,", ", C133,", ",D133,", ",E133, ",[",F133,"],'",G133,"'),")</f>
-        <v xml:space="preserve"> new Room('321', 125, 59, 9, 4,[4,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I133" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('317', 125, 51, 9, 4,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>168</v>
+        <v>85</v>
       </c>
       <c r="B134">
         <v>125</v>
       </c>
       <c r="C134">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D134">
         <v>9</v>
       </c>
       <c r="E134">
+        <v>4</v>
+      </c>
+      <c r="F134" t="s">
+        <v>181</v>
+      </c>
+      <c r="G134" t="s">
+        <v>166</v>
+      </c>
+      <c r="I134" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('319', 125, 55, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B135">
+        <v>125</v>
+      </c>
+      <c r="C135">
+        <v>59</v>
+      </c>
+      <c r="D135">
+        <v>9</v>
+      </c>
+      <c r="E135">
+        <v>4</v>
+      </c>
+      <c r="F135" t="s">
+        <v>198</v>
+      </c>
+      <c r="G135" t="s">
+        <v>166</v>
+      </c>
+      <c r="I135" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('321', 125, 59, 9, 4,[4,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B136">
+        <v>125</v>
+      </c>
+      <c r="C136">
+        <v>64</v>
+      </c>
+      <c r="D136">
+        <v>9</v>
+      </c>
+      <c r="E136">
         <v>3</v>
       </c>
-      <c r="F134" t="s">
-        <v>210</v>
-      </c>
-      <c r="G134" t="s">
-        <v>214</v>
-      </c>
-      <c r="H134" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> new Room('stairs2', 125, 64, 9, 3,[4,2,4,1],'Stair'),</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+      <c r="F136" t="s">
+        <v>209</v>
+      </c>
+      <c r="G136" t="s">
+        <v>213</v>
+      </c>
+      <c r="I136" t="str">
+        <f t="shared" si="14"/>
+        <v xml:space="preserve"> new Room('stairs2', 125, 64, 9, 3,[4,2,4,1],'Stair',''),</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B136">
+      <c r="B138">
         <v>103</v>
       </c>
-      <c r="C136">
+      <c r="C138">
         <v>33</v>
       </c>
-      <c r="D136">
+      <c r="D138">
         <v>10</v>
       </c>
-      <c r="E136">
-        <f>E137+E138+E139+E140</f>
+      <c r="E138">
+        <f>E139+E140+E141+E142</f>
         <v>10</v>
       </c>
-      <c r="G136" t="s">
-        <v>166</v>
-      </c>
-      <c r="H136" t="str">
-        <f>CONCATENATE(" new Room('", A136,"', ", B136,", ", C136,", ",D136,", ",E136, ",[",F136,"],'",G136,"'),")</f>
-        <v xml:space="preserve"> new Room('Courtyard5', 103, 33, 10, 10,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="G138" t="s">
+        <v>166</v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" ref="I138:I142" si="15">CONCATENATE(" new Room('", A138,"', ", B138,", ", C138,", ",D138,", ",E138, ",[",F138,"],'",G138,"','",H138,"'),")</f>
+        <v xml:space="preserve"> new Room('Courtyard5', 103, 33, 10, 10,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B137">
-        <v>113</v>
-      </c>
-      <c r="C137">
-        <v>33</v>
-      </c>
-      <c r="D137">
-        <v>9</v>
-      </c>
-      <c r="E137">
-        <v>2</v>
-      </c>
-      <c r="F137" t="s">
-        <v>200</v>
-      </c>
-      <c r="G137" t="s">
-        <v>166</v>
-      </c>
-      <c r="H137" t="str">
-        <f>CONCATENATE(" new Room('", A137,"', ", B137,", ", C137,", ",D137,", ",E137, ",[",F137,"],'",G137,"'),")</f>
-        <v xml:space="preserve"> new Room('boys br1', 113, 33, 9, 2,[2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="138" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B138">
-        <v>113</v>
-      </c>
-      <c r="C138">
-        <v>35</v>
-      </c>
-      <c r="D138">
-        <v>9</v>
-      </c>
-      <c r="E138">
-        <v>2</v>
-      </c>
-      <c r="F138" t="s">
-        <v>175</v>
-      </c>
-      <c r="G138" t="s">
-        <v>166</v>
-      </c>
-      <c r="H138" t="str">
-        <f>CONCATENATE(" new Room('", A138,"', ", B138,", ", C138,", ",D138,", ",E138, ",[",F138,"],'",G138,"'),")</f>
-        <v xml:space="preserve"> new Room('girls br1', 113, 35, 9, 2,[2,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="B139">
         <v>113</v>
       </c>
       <c r="C139">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D139">
         <v>9</v>
       </c>
       <c r="E139">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F139" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="G139" t="s">
         <v>166</v>
       </c>
-      <c r="H139" t="str">
-        <f>CONCATENATE(" new Room('", A139,"', ", B139,", ", C139,", ",D139,", ",E139, ",[",F139,"],'",G139,"'),")</f>
-        <v xml:space="preserve"> new Room('fake 322', 113, 37, 9, 3,[2,2],'Normal'),</v>
-      </c>
-    </row>
-    <row r="140" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I139" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> new Room('boys br1', 113, 33, 9, 2,[2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>73</v>
+        <v>161</v>
       </c>
       <c r="B140">
         <v>113</v>
       </c>
       <c r="C140">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D140">
         <v>9</v>
       </c>
       <c r="E140">
+        <v>2</v>
+      </c>
+      <c r="F140" t="s">
+        <v>175</v>
+      </c>
+      <c r="G140" t="s">
+        <v>166</v>
+      </c>
+      <c r="I140" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> new Room('girls br1', 113, 35, 9, 2,[2,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B141">
+        <v>113</v>
+      </c>
+      <c r="C141">
+        <v>37</v>
+      </c>
+      <c r="D141">
+        <v>9</v>
+      </c>
+      <c r="E141">
         <v>3</v>
       </c>
-      <c r="F140" t="s">
+      <c r="F141" t="s">
+        <v>175</v>
+      </c>
+      <c r="G141" t="s">
+        <v>166</v>
+      </c>
+      <c r="I141" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> new Room('309', 113, 37, 9, 3,[2,2],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B142">
+        <v>113</v>
+      </c>
+      <c r="C142">
+        <v>40</v>
+      </c>
+      <c r="D142">
+        <v>9</v>
+      </c>
+      <c r="E142">
+        <v>3</v>
+      </c>
+      <c r="F142" t="s">
         <v>176</v>
       </c>
-      <c r="G140" t="s">
-        <v>166</v>
-      </c>
-      <c r="H140" t="str">
-        <f>CONCATENATE(" new Room('", A140,"', ", B140,", ", C140,", ",D140,", ",E140, ",[",F140,"],'",G140,"'),")</f>
-        <v xml:space="preserve"> new Room('312', 113, 40, 9, 3,[2,3],'Normal'),</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="G142" t="s">
+        <v>166</v>
+      </c>
+      <c r="I142" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve"> new Room('312', 113, 40, 9, 3,[2,3],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B142">
+      <c r="B144">
         <v>103</v>
       </c>
-      <c r="C142">
+      <c r="C144">
         <v>45</v>
       </c>
-      <c r="D142">
+      <c r="D144">
         <v>10</v>
       </c>
-      <c r="E142">
-        <f>E143+E144</f>
+      <c r="E144">
+        <f>E145+E146</f>
         <v>8</v>
       </c>
-      <c r="G142" t="s">
-        <v>166</v>
-      </c>
-      <c r="H142" t="str">
-        <f>CONCATENATE(" new Room('", A142,"', ", B142,", ", C142,", ",D142,", ",E142, ",[",F142,"],'",G142,"'),")</f>
-        <v xml:space="preserve"> new Room('Courtyard4', 103, 45, 10, 8,[],'Normal'),</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="G144" t="s">
+        <v>166</v>
+      </c>
+      <c r="I144" t="str">
+        <f t="shared" ref="I144:I149" si="16">CONCATENATE(" new Room('", A144,"', ", B144,", ", C144,", ",D144,", ",E144, ",[",F144,"],'",G144,"','",H144,"'),")</f>
+        <v xml:space="preserve"> new Room('Courtyard4', 103, 45, 10, 8,[],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B143">
-        <v>113</v>
-      </c>
-      <c r="C143">
-        <v>45</v>
-      </c>
-      <c r="D143">
-        <v>9</v>
-      </c>
-      <c r="E143">
-        <v>4</v>
-      </c>
-      <c r="F143" t="s">
-        <v>177</v>
-      </c>
-      <c r="G143" t="s">
-        <v>166</v>
-      </c>
-      <c r="H143" t="str">
-        <f>CONCATENATE(" new Room('", A143,"', ", B143,", ", C143,", ",D143,", ",E143, ",[",F143,"],'",G143,"'),")</f>
-        <v xml:space="preserve"> new Room('314', 113, 45, 9, 4,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B144">
-        <v>113</v>
-      </c>
-      <c r="C144">
-        <v>49</v>
-      </c>
-      <c r="D144">
-        <v>9</v>
-      </c>
-      <c r="E144">
-        <v>4</v>
-      </c>
-      <c r="F144" t="s">
-        <v>200</v>
-      </c>
-      <c r="G144" t="s">
-        <v>166</v>
-      </c>
-      <c r="H144" t="str">
-        <f>CONCATENATE(" new Room('", A144,"', ", B144,", ", C144,", ",D144,", ",E144, ",[",F144,"],'",G144,"'),")</f>
-        <v xml:space="preserve"> new Room('316', 113, 49, 9, 4,[2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="B145">
         <v>113</v>
       </c>
       <c r="C145">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D145">
         <v>9</v>
@@ -7500,25 +7536,25 @@
         <v>4</v>
       </c>
       <c r="F145" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="G145" t="s">
         <v>166</v>
       </c>
-      <c r="H145" t="str">
-        <f>CONCATENATE(" new Room('", A145,"', ", B145,", ", C145,", ",D145,", ",E145, ",[",F145,"],'",G145,"'),")</f>
-        <v xml:space="preserve"> new Room('318', 113, 55, 9, 4,[2,1],'Normal'),</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I145" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve"> new Room('314', 113, 45, 9, 4,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B146">
         <v>113</v>
       </c>
       <c r="C146">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D146">
         <v>9</v>
@@ -7527,42 +7563,96 @@
         <v>4</v>
       </c>
       <c r="F146" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="G146" t="s">
         <v>166</v>
       </c>
-      <c r="H146" t="str">
-        <f>CONCATENATE(" new Room('", A146,"', ", B146,", ", C146,", ",D146,", ",E146, ",[",F146,"],'",G146,"'),")</f>
-        <v xml:space="preserve"> new Room('320', 113, 59, 9, 4,[2,4],'Normal'),</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I146" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve"> new Room('316', 113, 49, 9, 4,[2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B147">
         <v>113</v>
       </c>
       <c r="C147">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D147">
         <v>9</v>
       </c>
       <c r="E147">
-        <f>E146</f>
         <v>4</v>
       </c>
       <c r="F147" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G147" t="s">
         <v>166</v>
       </c>
-      <c r="H147" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> new Room('322', 113, 63, 9, 4,[2,1],'Normal'),</v>
+      <c r="I147" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve"> new Room('318', 113, 55, 9, 4,[2,1],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B148">
+        <v>113</v>
+      </c>
+      <c r="C148">
+        <v>59</v>
+      </c>
+      <c r="D148">
+        <v>9</v>
+      </c>
+      <c r="E148">
+        <v>4</v>
+      </c>
+      <c r="F148" t="s">
+        <v>177</v>
+      </c>
+      <c r="G148" t="s">
+        <v>166</v>
+      </c>
+      <c r="I148" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve"> new Room('320', 113, 59, 9, 4,[2,4],'Normal',''),</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B149">
+        <v>113</v>
+      </c>
+      <c r="C149">
+        <v>63</v>
+      </c>
+      <c r="D149">
+        <v>9</v>
+      </c>
+      <c r="E149">
+        <f>E148</f>
+        <v>4</v>
+      </c>
+      <c r="F149" t="s">
+        <v>199</v>
+      </c>
+      <c r="G149" t="s">
+        <v>166</v>
+      </c>
+      <c r="I149" t="str">
+        <f t="shared" si="16"/>
+        <v xml:space="preserve"> new Room('322', 113, 63, 9, 4,[2,1],'Normal',''),</v>
       </c>
     </row>
   </sheetData>
@@ -7576,18 +7666,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I2:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>113</v>
       </c>
@@ -7609,11 +7699,14 @@
       <c r="G1" t="s">
         <v>172</v>
       </c>
-      <c r="K1" t="s">
+      <c r="H1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>122</v>
       </c>
@@ -7630,22 +7723,22 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G2" t="s">
         <v>166</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE(" new Room('", A2,"', ", B2,", ", C2,", ",D2,", ",E2, ",[",F2,"],'",G2,"'),")</f>
-        <v xml:space="preserve"> new Room('Boys BR', 0, 0, 8, 2,[2,1],'Normal'),</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="I2" t="str">
+        <f>CONCATENATE(" new Room('", A2,"', ", B2,", ", C2,", ",D2,", ",E2, ",[",F2,"],'",G2,"','",H2,"'),")</f>
+        <v xml:space="preserve"> new Room('Boys BR', 0, 0, 8, 2,[2,1],'Normal',''),</v>
+      </c>
+      <c r="L2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7661,20 +7754,20 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G3" t="s">
         <v>166</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H22" si="0">CONCATENATE(" new Room('", A3,"', ", B3,", ", C3,", ",D3,", ",E3, ",[",F3,"],'",G3,"'),")</f>
-        <v xml:space="preserve"> new Room('girls BR', 0, 2, 8, 2,[2,1],'Normal'),</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I11" si="0">CONCATENATE(" new Room('", A3,"', ", B3,", ", C3,", ",D3,", ",E3, ",[",F3,"],'",G3,"','",H3,"'),")</f>
+        <v xml:space="preserve"> new Room('Girls BR', 0, 2, 8, 2,[2,1],'Normal',''),</v>
+      </c>
+      <c r="L3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -7697,15 +7790,15 @@
       <c r="G4" t="s">
         <v>166</v>
       </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('workroom', 0, 4, 8, 5,[2,3],'Normal'),</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('workroom', 0, 4, 8, 5,[2,3],'Normal',''),</v>
+      </c>
+      <c r="L4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>412</v>
       </c>
@@ -7728,15 +7821,15 @@
       <c r="G5" t="s">
         <v>166</v>
       </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('412', 0, 9, 8, 4,[2,4],'Normal'),</v>
-      </c>
-      <c r="K5">
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('412', 0, 9, 8, 4,[2,4],'Normal',''),</v>
+      </c>
+      <c r="L5">
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>414</v>
       </c>
@@ -7754,20 +7847,20 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G6" t="s">
         <v>166</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('414', 0, 13, 8, 4,[2,1],'Normal'),</v>
-      </c>
-      <c r="K6">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('414', 0, 13, 8, 4,[2,1],'Normal',''),</v>
+      </c>
+      <c r="L6">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>416</v>
       </c>
@@ -7790,15 +7883,15 @@
       <c r="G7" t="s">
         <v>166</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('416', 0, 17, 8, 4,[2,4],'Normal'),</v>
-      </c>
-      <c r="K7">
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('416', 0, 17, 8, 4,[2,4],'Normal',''),</v>
+      </c>
+      <c r="L7">
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>418</v>
       </c>
@@ -7816,20 +7909,20 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G8" t="s">
         <v>166</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('418', 0, 21, 8, 4,[2,1],'Normal'),</v>
-      </c>
-      <c r="K8">
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('418', 0, 21, 8, 4,[2,1],'Normal',''),</v>
+      </c>
+      <c r="L8">
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>420</v>
       </c>
@@ -7852,15 +7945,15 @@
       <c r="G9" t="s">
         <v>166</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('420', 0, 25, 8, 4,[2,4],'Normal'),</v>
-      </c>
-      <c r="K9">
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('420', 0, 25, 8, 4,[2,4],'Normal',''),</v>
+      </c>
+      <c r="L9">
         <v>173</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>422</v>
       </c>
@@ -7878,22 +7971,22 @@
         <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G10" t="s">
         <v>166</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('422', 0, 29, 8, 4,[2,1],'Normal'),</v>
-      </c>
-      <c r="K10">
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('422', 0, 29, 8, 4,[2,1],'Normal',''),</v>
+      </c>
+      <c r="L10">
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>215</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -7911,17 +8004,17 @@
       <c r="G11" t="s">
         <v>166</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Storage', 0, 33, 8, 3,[],'Normal'),</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Room('Storage1', 0, 33, 8, 3,[],'Normal',''),</v>
+      </c>
+      <c r="L11" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -7936,20 +8029,20 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G13" t="s">
-        <v>214</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('stairs1', 12, 0, 9, 2,[4,1,4,2],'Stair'),</v>
-      </c>
-      <c r="K13" t="s">
+        <v>213</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ref="I13:I22" si="2">CONCATENATE(" new Room('", A13,"', ", B13,", ", C13,", ",D13,", ",E13, ",[",F13,"],'",G13,"','",H13,"'),")</f>
+        <v xml:space="preserve"> new Room('Stairs1', 12, 0, 9, 2,[4,1,4,2],'Stair',''),</v>
+      </c>
+      <c r="L13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -7967,20 +8060,20 @@
         <v>5</v>
       </c>
       <c r="F14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G14" t="s">
         <v>166</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('Workroom', 12, 2, 9, 5,[4,3],'Normal'),</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="I14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('Workroom', 12, 2, 9, 5,[4,3],'Normal',''),</v>
+      </c>
+      <c r="L14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>411</v>
       </c>
@@ -7988,7 +8081,7 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C22" si="2">C14+E14</f>
+        <f t="shared" ref="C15:C22" si="3">C14+E14</f>
         <v>7</v>
       </c>
       <c r="D15">
@@ -7998,20 +8091,20 @@
         <v>4</v>
       </c>
       <c r="F15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G15" t="s">
+        <v>166</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('411', 12, 7, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+      <c r="L15">
         <v>182</v>
       </c>
-      <c r="G15" t="s">
-        <v>166</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('411', 12, 7, 9, 4,[4,4],'Normal'),</v>
-      </c>
-      <c r="K15">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>413</v>
       </c>
@@ -8019,7 +8112,7 @@
         <v>12</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="D16">
@@ -8029,20 +8122,20 @@
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G16" t="s">
         <v>166</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('413', 12, 11, 9, 4,[4,1],'Normal'),</v>
-      </c>
-      <c r="K16">
+      <c r="I16" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('413', 12, 11, 9, 4,[4,1],'Normal',''),</v>
+      </c>
+      <c r="L16">
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>415</v>
       </c>
@@ -8050,7 +8143,7 @@
         <v>12</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="D17">
@@ -8060,20 +8153,20 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G17" t="s">
         <v>166</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('415', 12, 15, 9, 4,[4,4],'Normal'),</v>
-      </c>
-      <c r="K17">
+      <c r="I17" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('415', 12, 15, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+      <c r="L17">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>417</v>
       </c>
@@ -8081,7 +8174,7 @@
         <v>12</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="D18">
@@ -8091,20 +8184,20 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G18" t="s">
         <v>166</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('417', 12, 19, 9, 3,[4,1],'Normal'),</v>
-      </c>
-      <c r="K18">
+      <c r="I18" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('417', 12, 19, 9, 3,[4,1],'Normal',''),</v>
+      </c>
+      <c r="L18">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>419</v>
       </c>
@@ -8112,7 +8205,7 @@
         <v>12</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="D19">
@@ -8122,20 +8215,20 @@
         <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G19" t="s">
         <v>166</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('419', 12, 22, 9, 4,[4,4],'Normal'),</v>
-      </c>
-      <c r="K19">
+      <c r="I19" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('419', 12, 22, 9, 4,[4,4],'Normal',''),</v>
+      </c>
+      <c r="L19">
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>421</v>
       </c>
@@ -8143,7 +8236,7 @@
         <v>12</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D20">
@@ -8153,28 +8246,28 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G20" t="s">
         <v>166</v>
       </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('421', 12, 26, 9, 3,[4,1],'Normal'),</v>
-      </c>
-      <c r="K20">
+      <c r="I20" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('421', 12, 26, 9, 3,[4,1],'Normal',''),</v>
+      </c>
+      <c r="L20">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>12</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="D21">
@@ -8184,28 +8277,28 @@
         <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G21" t="s">
         <v>166</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('storage', 12, 29, 9, 3,[4,4],'Normal'),</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="I21" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('Storage', 12, 29, 9, 3,[4,4],'Normal',''),</v>
+      </c>
+      <c r="L21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="B22">
         <v>12</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="D22">
@@ -8215,16 +8308,16 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G22" t="s">
-        <v>214</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Room('stairs2', 12, 32, 8, 2,[4,1,4,2],'Stair'),</v>
-      </c>
-      <c r="K22" t="s">
+        <v>213</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve"> new Room('Stairs2', 12, 32, 8, 2,[4,1,4,2],'Stair',''),</v>
+      </c>
+      <c r="L22" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>